<commit_message>
Update with latest modelling
</commit_message>
<xml_diff>
--- a/Correspondence Tables/ELMO/ELMO-EDC Correspondence.xlsx
+++ b/Correspondence Tables/ELMO/ELMO-EDC Correspondence.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Repositories\EDCI-Data-Model\Correspondence Models\ELMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Repos\prelaunch\Correspondence Tables\ELMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30BBF480-48FB-4454-AEF8-AE6B9AA13D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BC055-F9D7-4726-B7B0-535F88C91AF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3FC7D471-8EE2-4B15-AE53-6C073BB5F682}"/>
   </bookViews>

</xml_diff>